<commit_message>
Update data.json and report checklist - test 11,12
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GEHEALTHCARE/GEMSI/CENTRICITYRIS/7/report_checklist.xlsx
+++ b/GATEWAY/A1#111GEHEALTHCARE/GEMSI/CENTRICITYRIS/7/report_checklist.xlsx
@@ -379,13 +379,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-31T12:04:13Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2e68c3c8c5ba061a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.99999.794d23f121b3a3803b7bd202128e298410c49b59b5d7ad680bc56318a5ff53cb.35d16048ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-08-01T09:30:57Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48c68cf29d03bb0d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.99999.794d23f121b3a3803b7bd202128e298410c49b59b5d7ad680bc56318a5ff53cb.f7f48ec24e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -399,13 +399,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-31T12:06:41Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4b35485cae8e9515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.99999.794d23f121b3a3803b7bd202128e298410c49b59b5d7ad680bc56318a5ff53cb.9cbe71424e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-08-01T09:37:02Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48c678f71be069fa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.99999.794d23f121b3a3803b7bd202128e298410c49b59b5d7ad680bc56318a5ff53cb.bb9e8e1a65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT3</t>
@@ -4710,7 +4710,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.82"/>
@@ -5784,7 +5784,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.09"/>
@@ -6889,13 +6889,13 @@
   </sheetPr>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="F7" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="topRight" activeCell="G21" activeCellId="0" sqref="G21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.83"/>
@@ -7468,7 +7468,7 @@
         <v>72</v>
       </c>
       <c r="F19" s="27" t="n">
-        <v>45138</v>
+        <v>45139</v>
       </c>
       <c r="G19" s="33" t="s">
         <v>73</v>
@@ -7512,7 +7512,7 @@
         <v>78</v>
       </c>
       <c r="F20" s="27" t="n">
-        <v>45138</v>
+        <v>45139</v>
       </c>
       <c r="G20" s="28" t="s">
         <v>79</v>
@@ -24913,7 +24913,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.91"/>
@@ -26594,7 +26594,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.09"/>

</xml_diff>